<commit_message>
Updated BOMs, added images
added more details in BOM and pics of boards
</commit_message>
<xml_diff>
--- a/2HPico KiCad design files/Pico 2HP Controls/Pico2HP Controls BOM.xlsx
+++ b/2HPico KiCad design files/Pico 2HP Controls/Pico2HP Controls BOM.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Pico_2HP_Controls" localSheetId="0">Sheet1!$A$1:$H$7</definedName>
+    <definedName name="Pico_2HP_Controls" localSheetId="0">Sheet1!$A$1:$H$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Id</t>
   </si>
@@ -58,12 +58,6 @@
     <t>Supplier and ref</t>
   </si>
   <si>
-    <t>J3,J1,J2</t>
-  </si>
-  <si>
-    <t>Conn_01x04_Pin</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
     <t>SW_PUSH_6mm (13mm shaft)</t>
   </si>
   <si>
-    <t>PinHeader_1x04_P2.54mm_R/A</t>
-  </si>
-  <si>
     <t>LED_OPSCO_SK6812_MINI-E_3228SMD Reverse Mount</t>
   </si>
   <si>
@@ -154,23 +145,20 @@
     <t xml:space="preserve">Knobs to fit pots </t>
   </si>
   <si>
-    <t>these are in the main board BOM - don't buy 2 sets</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.com/item/33009959086.html</t>
   </si>
   <si>
-    <t>do NOT use metal pots - the frame will short the board connectors</t>
-  </si>
-  <si>
     <t>10k to 100k is fine - could also use Song Huei style plastic pots with pointer on shaft</t>
+  </si>
+  <si>
+    <t>***** do NOT use metal pots - the frame will short the board connectors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +170,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -208,9 +204,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -224,6 +221,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1932990</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>37595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5210175" y="2095500"/>
+          <a:ext cx="4676190" cy="4038095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -517,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,10 +595,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -569,16 +609,22 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
-        <v>38</v>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -592,19 +638,19 @@
         <v>22</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -615,22 +661,22 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -638,25 +684,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -664,42 +701,42 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
         <v>33</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -707,48 +744,32 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
-    <hyperlink ref="G5" r:id="rId3"/>
-    <hyperlink ref="G8" r:id="rId4"/>
-    <hyperlink ref="G7" r:id="rId5"/>
-    <hyperlink ref="G9" r:id="rId6"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G7" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>